<commit_message>
calculo menstru sep 21
</commit_message>
<xml_diff>
--- a/MenstruAccion/cuanto_cuesta_menstruar/2021 Septiembre/Fuentes/serie_precios_pgm.xlsx
+++ b/MenstruAccion/cuanto_cuesta_menstruar/2021 Septiembre/Fuentes/serie_precios_pgm.xlsx
@@ -212,13 +212,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
+      <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -284,6 +284,17 @@
       </c>
       <c r="C6" s="0" t="n">
         <v>14.59</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="2" t="n">
+        <v>44440</v>
+      </c>
+      <c r="B7" s="0" t="n">
+        <v>14.34</v>
+      </c>
+      <c r="C7" s="0" t="n">
+        <v>16.38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>